<commit_message>
update key value and  add NA-> Rohit
</commit_message>
<xml_diff>
--- a/keyValue.xlsx
+++ b/keyValue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit_PC\Downloads\csv\rohit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit_PC\Documents\GitHub\CleanUpTardeDataCsv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10B5162-7D7B-4608-8C9B-6D677535D064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270B624C-E7D5-483C-AA4F-C0656C90E894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{545FE23A-181C-40B4-A429-5355ED4BAF6A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="keyValue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_2" localSheetId="0" hidden="1">keyValue!$A$1:$B$150</definedName>
+    <definedName name="ExternalData_2" localSheetId="0" hidden="1">keyValue!$A$1:$B$152</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="295">
   <si>
     <t>ZYDUSWELL.NS</t>
   </si>
@@ -912,6 +912,18 @@
   </si>
   <si>
     <t>Nippon India Nifty Next 50 ETF</t>
+  </si>
+  <si>
+    <t>Adani Power</t>
+  </si>
+  <si>
+    <t>Cochin Shipyard</t>
+  </si>
+  <si>
+    <t>ADANIPOWER.NS</t>
+  </si>
+  <si>
+    <t>COCHINSHIP.NS</t>
   </si>
 </sst>
 </file>
@@ -947,9 +959,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -992,10 +1008,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90CF6DDF-62D9-4114-842E-90BBCDD39181}" name="keyValue" displayName="keyValue" ref="A1:B150" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B150" xr:uid="{CBA618BA-7BE1-4E38-8E4A-65CA99CAFE3F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B150">
-    <sortCondition ref="A1:A150"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90CF6DDF-62D9-4114-842E-90BBCDD39181}" name="keyValue" displayName="keyValue" ref="A1:B152" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B152" xr:uid="{CBA618BA-7BE1-4E38-8E4A-65CA99CAFE3F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B152">
+    <sortCondition ref="A1:A152"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3599B9FA-BFE5-42CC-BB2B-CEBD2197B4A3}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="1"/>
@@ -1302,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6CE9B2-1CFD-45AA-9BDA-0446C562F115}">
-  <dimension ref="A1:B150"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,456 +1364,456 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B5" t="s">
-        <v>259</v>
+      <c r="A5" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B16" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B23" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>277</v>
+        <v>216</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>213</v>
+        <v>277</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B36" t="s">
-        <v>202</v>
+      <c r="A36" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>284</v>
+        <v>203</v>
       </c>
       <c r="B38" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>197</v>
+        <v>284</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>285</v>
+        <v>160</v>
       </c>
       <c r="B61" t="s">
         <v>159</v>
@@ -1805,39 +1821,39 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>152</v>
+        <v>285</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>286</v>
+        <v>154</v>
       </c>
       <c r="B66" t="s">
         <v>153</v>
@@ -1845,7 +1861,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>288</v>
+        <v>150</v>
       </c>
       <c r="B67" t="s">
         <v>149</v>
@@ -1853,223 +1869,223 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>148</v>
+        <v>286</v>
       </c>
       <c r="B68" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>288</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>272</v>
+        <v>134</v>
       </c>
       <c r="B76" t="s">
-        <v>271</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>130</v>
+        <v>272</v>
       </c>
       <c r="B78" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B86" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="B95" t="s">
         <v>98</v>
@@ -2077,7 +2093,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>287</v>
+        <v>100</v>
       </c>
       <c r="B96" t="s">
         <v>99</v>
@@ -2085,433 +2101,449 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>97</v>
+        <v>273</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>276</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>94</v>
+        <v>279</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>92</v>
+        <v>276</v>
       </c>
       <c r="B101" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>290</v>
+        <v>92</v>
       </c>
       <c r="B103" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>86</v>
+        <v>290</v>
       </c>
       <c r="B105" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B109" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B113" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B114" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B115" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B116" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B117" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B118" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B119" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>269</v>
+        <v>58</v>
       </c>
       <c r="B121" t="s">
-        <v>270</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="B123" t="s">
-        <v>51</v>
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B124" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B125" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B126" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B127" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B128" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B129" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B130" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B131" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B132" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B133" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>278</v>
+        <v>40</v>
       </c>
       <c r="B135" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>282</v>
+        <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>283</v>
+        <v>29</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>27</v>
+        <v>278</v>
       </c>
       <c r="B137" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>25</v>
+        <v>282</v>
       </c>
       <c r="B138" t="s">
-        <v>24</v>
+        <v>283</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B139" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B140" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B142" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B144" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B145" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B146" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B152" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add special case in icici etf and bank
</commit_message>
<xml_diff>
--- a/keyValue.xlsx
+++ b/keyValue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit_PC\Documents\GitHub\CleanUpTardeDataCsv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AA144F-EFC6-4192-9F12-5D735B53C59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711A9259-6A06-4D45-B201-6111E638C936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{545FE23A-181C-40B4-A429-5355ED4BAF6A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="keyValue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_2" localSheetId="0" hidden="1">keyValue!$A$1:$B$177</definedName>
+    <definedName name="ExternalData_2" localSheetId="0" hidden="1">keyValue!$A$1:$B$184</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="360">
   <si>
     <t>ZYDUSWELL.NS</t>
   </si>
@@ -494,9 +494,6 @@
     <t>ICICI Prudential IT ETF</t>
   </si>
   <si>
-    <t>ICICIBANKN.NS</t>
-  </si>
-  <si>
     <t>ICICI Pru Bank Nifty ETF</t>
   </si>
   <si>
@@ -899,9 +896,6 @@
     <t>HUL Hindustan Unilever</t>
   </si>
   <si>
-    <t>ICICI Prudential Nifty ETF</t>
-  </si>
-  <si>
     <t>Motilal Oswal Nifty Midcap 100</t>
   </si>
   <si>
@@ -1074,6 +1068,57 @@
   </si>
   <si>
     <t>NFL.NS</t>
+  </si>
+  <si>
+    <t>Exide Industries</t>
+  </si>
+  <si>
+    <t>EXIDEIND.NS</t>
+  </si>
+  <si>
+    <t>Amara Raja Energy &amp; Mobility</t>
+  </si>
+  <si>
+    <t>ARE&amp;M.NS</t>
+  </si>
+  <si>
+    <t>GE Power</t>
+  </si>
+  <si>
+    <t>GEPIL.NS</t>
+  </si>
+  <si>
+    <t>BLS International Services</t>
+  </si>
+  <si>
+    <t>BLS.NS</t>
+  </si>
+  <si>
+    <t>ABDL.NS</t>
+  </si>
+  <si>
+    <t>Allied Blenders and Distillers Limited</t>
+  </si>
+  <si>
+    <t>Shipping Corporation of India</t>
+  </si>
+  <si>
+    <t>SCI.NS</t>
+  </si>
+  <si>
+    <t>Federal Bank</t>
+  </si>
+  <si>
+    <t>FEDERALBNK.NS</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Nifty Bank ETF</t>
+  </si>
+  <si>
+    <t>rohit bank1</t>
+  </si>
+  <si>
+    <t>rohit bank2</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1199,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90CF6DDF-62D9-4114-842E-90BBCDD39181}" name="keyValue" displayName="keyValue" ref="A1:B177" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B177" xr:uid="{CBA618BA-7BE1-4E38-8E4A-65CA99CAFE3F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B153">
-    <sortCondition ref="A1:A153"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90CF6DDF-62D9-4114-842E-90BBCDD39181}" name="keyValue" displayName="keyValue" ref="A1:B184" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B184" xr:uid="{CBA618BA-7BE1-4E38-8E4A-65CA99CAFE3F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B177">
+    <sortCondition ref="A1:A177"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3599B9FA-BFE5-42CC-BB2B-CEBD2197B4A3}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="1"/>
@@ -1464,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6CE9B2-1CFD-45AA-9BDA-0446C562F115}">
-  <dimension ref="A1:B177"/>
+  <dimension ref="A1:B184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1479,63 +1524,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>295</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" t="s">
         <v>262</v>
-      </c>
-      <c r="B5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>291</v>
+        <v>261</v>
       </c>
       <c r="B6" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B8" t="s">
         <v>258</v>
@@ -1543,1354 +1588,1410 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" t="s">
         <v>257</v>
-      </c>
-      <c r="B9" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" t="s">
         <v>255</v>
-      </c>
-      <c r="B10" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>253</v>
+        <v>311</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B20" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B23" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>228</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
-        <v>227</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>226</v>
+        <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B27" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B30" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>277</v>
+        <v>331</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>330</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="B34" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>292</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>294</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B38" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>201</v>
+        <v>338</v>
       </c>
       <c r="B40" t="s">
-        <v>200</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>284</v>
+        <v>212</v>
       </c>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="B42" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>193</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B50" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="B52" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B53" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>177</v>
+        <v>321</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>169</v>
+        <v>315</v>
       </c>
       <c r="B57" t="s">
-        <v>168</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>285</v>
+        <v>172</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B65" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="B68" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>286</v>
+        <v>164</v>
       </c>
       <c r="B69" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>288</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>140</v>
+        <v>297</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>138</v>
+        <v>284</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>134</v>
+        <v>357</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>141</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>272</v>
+        <v>153</v>
       </c>
       <c r="B79" t="s">
-        <v>271</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>130</v>
+        <v>302</v>
       </c>
       <c r="B81" t="s">
-        <v>129</v>
+        <v>301</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B88" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>309</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>289</v>
+        <v>126</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>273</v>
+        <v>122</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>287</v>
+        <v>120</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>279</v>
+        <v>116</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>276</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B105" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>290</v>
+        <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>88</v>
+        <v>328</v>
       </c>
       <c r="B107" t="s">
-        <v>87</v>
+        <v>329</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>84</v>
+        <v>323</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
+        <v>324</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>82</v>
+        <v>326</v>
       </c>
       <c r="B110" t="s">
-        <v>81</v>
+        <v>327</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>78</v>
+        <v>287</v>
       </c>
       <c r="B112" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B113" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>74</v>
+        <v>272</v>
       </c>
       <c r="B114" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>72</v>
+        <v>285</v>
       </c>
       <c r="B115" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>70</v>
+        <v>295</v>
       </c>
       <c r="B116" t="s">
-        <v>69</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>68</v>
+        <v>341</v>
       </c>
       <c r="B117" t="s">
-        <v>67</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="B118" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>64</v>
+        <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>62</v>
+        <v>275</v>
       </c>
       <c r="B120" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B121" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B122" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B123" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="B124" t="s">
-        <v>270</v>
+        <v>89</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B125" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B126" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B127" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="B128" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B129" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B130" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B131" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B132" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="B133" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="B134" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B135" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B136" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B137" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>282</v>
+        <v>60</v>
       </c>
       <c r="B139" t="s">
-        <v>283</v>
+        <v>59</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>27</v>
+        <v>325</v>
       </c>
       <c r="B140" t="s">
-        <v>26</v>
+        <v>334</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>25</v>
+        <v>339</v>
       </c>
       <c r="B141" t="s">
-        <v>24</v>
+        <v>340</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B142" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B143" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>19</v>
+        <v>268</v>
       </c>
       <c r="B144" t="s">
-        <v>18</v>
+        <v>269</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B145" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B146" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>13</v>
+        <v>319</v>
       </c>
       <c r="B147" t="s">
-        <v>12</v>
+        <v>320</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B148" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>9</v>
+        <v>299</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B152" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B153" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>297</v>
+        <v>38</v>
       </c>
       <c r="B154" t="s">
-        <v>298</v>
+        <v>37</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>299</v>
+        <v>36</v>
       </c>
       <c r="B155" t="s">
-        <v>300</v>
+        <v>35</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>301</v>
+        <v>34</v>
       </c>
       <c r="B156" t="s">
-        <v>302</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B157" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>305</v>
+        <v>32</v>
       </c>
       <c r="B158" t="s">
-        <v>306</v>
+        <v>31</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="B159" t="s">
-        <v>308</v>
+        <v>39</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>309</v>
+        <v>30</v>
       </c>
       <c r="B160" t="s">
-        <v>310</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="B161" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="B162" t="s">
-        <v>314</v>
+        <v>28</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="B163" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>317</v>
+        <v>27</v>
       </c>
       <c r="B164" t="s">
-        <v>318</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>319</v>
+        <v>25</v>
       </c>
       <c r="B165" t="s">
-        <v>320</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>321</v>
+        <v>23</v>
       </c>
       <c r="B166" t="s">
-        <v>322</v>
+        <v>22</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>323</v>
+        <v>21</v>
       </c>
       <c r="B167" t="s">
-        <v>324</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>325</v>
+        <v>19</v>
       </c>
       <c r="B168" t="s">
-        <v>326</v>
+        <v>18</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>327</v>
+        <v>17</v>
       </c>
       <c r="B169" t="s">
-        <v>336</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>328</v>
+        <v>15</v>
       </c>
       <c r="B170" t="s">
-        <v>329</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>330</v>
+        <v>13</v>
       </c>
       <c r="B171" t="s">
-        <v>331</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>333</v>
+        <v>11</v>
       </c>
       <c r="B172" t="s">
-        <v>332</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>334</v>
+        <v>9</v>
       </c>
       <c r="B173" t="s">
-        <v>335</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>337</v>
+        <v>7</v>
       </c>
       <c r="B174" t="s">
-        <v>338</v>
+        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>340</v>
+        <v>5</v>
       </c>
       <c r="B175" t="s">
-        <v>339</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>341</v>
+        <v>3</v>
       </c>
       <c r="B176" t="s">
-        <v>342</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B177" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B178" t="s">
         <v>344</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B179" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B180" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B181" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B182" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B183" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B184" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>